<commit_message>
Added Dam's Foal Search; Updated Graded Stakes for 2025 (GRCW-842)
</commit_message>
<xml_diff>
--- a/pdf/RTTBC25-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC25-Schedule-by-Division.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1162" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCB85305-DD73-4371-80B5-00D4ACF099BD}"/>
+  <xr:revisionPtr revIDLastSave="1166" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE751561-2066-4B69-B288-B084952CB9D3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
+    <workbookView xWindow="10620" yWindow="0" windowWidth="27690" windowHeight="20985" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -505,7 +505,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,6 +530,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -663,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -733,9 +739,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,6 +803,129 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,21 +933,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -830,110 +941,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -955,10 +973,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1258,16 +1272,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1783450-6415-4D0D-A0B8-DEE615502A89}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26:I28"/>
+      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1278,73 +1292,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="78"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="92" t="s">
+      <c r="A1" s="51"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="31" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="30" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="77"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="32" t="s">
+      <c r="A3" s="70"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="31" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="77"/>
-      <c r="B4" s="67">
+      <c r="A4" s="70"/>
+      <c r="B4" s="55">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1353,49 +1367,49 @@
       <c r="D4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
       <c r="G4" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="51"/>
+      <c r="H4" s="52"/>
       <c r="I4" s="9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="77"/>
-      <c r="B5" s="70"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="74"/>
-      <c r="H5" s="52"/>
+      <c r="H5" s="53"/>
       <c r="I5" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="77"/>
-      <c r="B6" s="68"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
       <c r="G6" s="75"/>
-      <c r="H6" s="53"/>
+      <c r="H6" s="54"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="77"/>
-      <c r="B7" s="35">
+      <c r="A7" s="70"/>
+      <c r="B7" s="34">
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
@@ -1411,8 +1425,8 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="77"/>
-      <c r="B8" s="35">
+      <c r="A8" s="70"/>
+      <c r="B8" s="34">
         <v>3</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -1427,737 +1441,719 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="77"/>
-      <c r="B9" s="67">
+    <row r="9" spans="1:9" s="93" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="70"/>
+      <c r="B9" s="40">
         <v>4</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="64" t="s">
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="37" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="77"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="66"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="77"/>
-      <c r="B11" s="67">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="70"/>
+      <c r="B10" s="55">
         <v>5</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="38" t="s">
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="I10" s="76" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="77"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="10" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="70"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="10" t="s">
         <v>99</v>
       </c>
+      <c r="D11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="83"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="70"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D12" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="83"/>
+    </row>
+    <row r="13" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="70"/>
+      <c r="B13" s="34">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="70"/>
+      <c r="B14" s="55">
+        <v>7</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="52"/>
+    </row>
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="70"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="84"/>
+      <c r="I15" s="53"/>
+    </row>
+    <row r="16" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="70"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="54"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="70"/>
+      <c r="B17" s="55">
+        <v>8</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="70"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="83"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="70"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A20" s="70"/>
+      <c r="B20" s="55">
+        <v>9</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="73" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="52"/>
+      <c r="F20" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="52"/>
+      <c r="H20" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" s="52"/>
+    </row>
+    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="70"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="74"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="83"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="53"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="70"/>
+      <c r="B22" s="55">
+        <v>10</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+    </row>
+    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="70"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="77"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="54"/>
+    </row>
+    <row r="24" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="70"/>
+      <c r="B24" s="40">
+        <v>11</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A25" s="70"/>
+      <c r="B25" s="55">
+        <v>12</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="52"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="52"/>
+    </row>
+    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A26" s="70"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="72"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I26" s="53"/>
+    </row>
+    <row r="27" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="70"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I27" s="54"/>
+    </row>
+    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A28" s="70"/>
+      <c r="B28" s="55">
+        <v>13</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="71" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="G28" s="52"/>
+      <c r="H28" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="I28" s="52"/>
+    </row>
+    <row r="29" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="70"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="77"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="54"/>
+    </row>
+    <row r="30" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="70"/>
+      <c r="B30" s="34">
+        <v>14</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="70"/>
+      <c r="B31" s="34">
         <v>15</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="65"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="77"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="65"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="65"/>
-    </row>
-    <row r="14" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="77"/>
-      <c r="B14" s="35">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="77"/>
-      <c r="B15" s="67">
-        <v>7</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="51"/>
-    </row>
-    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A16" s="77"/>
-      <c r="B16" s="70"/>
-      <c r="C16" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="52"/>
-    </row>
-    <row r="17" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="77"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="53"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="77"/>
-      <c r="B18" s="67">
-        <v>8</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="77"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="77"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A21" s="77"/>
-      <c r="B21" s="67">
-        <v>9</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="51"/>
-      <c r="F21" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="51"/>
-      <c r="H21" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="I21" s="51"/>
-    </row>
-    <row r="22" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="77"/>
-      <c r="B22" s="70"/>
-      <c r="C22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="74"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="52"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="77"/>
-      <c r="B23" s="67">
-        <v>10</v>
-      </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-    </row>
-    <row r="24" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="77"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="66"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-    </row>
-    <row r="25" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="77"/>
-      <c r="B25" s="41">
-        <v>11</v>
-      </c>
-      <c r="C25" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="77"/>
-      <c r="B26" s="67">
-        <v>12</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="58" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="51"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I26" s="51"/>
-    </row>
-    <row r="27" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A27" s="77"/>
-      <c r="B27" s="70"/>
-      <c r="C27" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I27" s="52"/>
-    </row>
-    <row r="28" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="77"/>
-      <c r="B28" s="68"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H28" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="I28" s="53"/>
-    </row>
-    <row r="29" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A29" s="77"/>
-      <c r="B29" s="67">
-        <v>13</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="64" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" s="51"/>
-      <c r="H29" s="64" t="s">
-        <v>105</v>
-      </c>
-      <c r="I29" s="51"/>
-    </row>
-    <row r="30" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="77"/>
-      <c r="B30" s="68"/>
-      <c r="C30" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="53"/>
-    </row>
-    <row r="31" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="77"/>
-      <c r="B31" s="35">
-        <v>14</v>
-      </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>56</v>
+      <c r="D31" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>59</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="77"/>
-      <c r="B32" s="35">
-        <v>15</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="F32" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A33" s="77"/>
-      <c r="B33" s="67">
+    <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A32" s="70"/>
+      <c r="B32" s="55">
         <v>16</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C32" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="58" t="s">
+      <c r="D32" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="61"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="38" t="s">
+      <c r="E32" s="85"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="I33" s="54" t="s">
+      <c r="I32" s="78" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="77"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="7" t="s">
+    <row r="33" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="70"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="59"/>
-      <c r="E34" s="62"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="86"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="I33" s="84"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="70"/>
+      <c r="B34" s="55">
+        <v>17</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="52"/>
       <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="I34" s="55"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="77"/>
-      <c r="B35" s="67">
-        <v>17</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" s="88" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="90" t="s">
+      <c r="G34" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="H35" s="54" t="s">
+      <c r="H34" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A36" s="77"/>
-      <c r="B36" s="70"/>
-      <c r="C36" s="19" t="s">
+    <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A35" s="70"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="89"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="91"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="56" t="s">
+      <c r="D35" s="65"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="84"/>
+      <c r="I35" s="91" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="77"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="47" t="s">
+    <row r="36" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="70"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D37" s="89"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="91"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="56"/>
-    </row>
-    <row r="38" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="77"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="10" t="s">
+      <c r="D36" s="65"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="84"/>
+      <c r="I36" s="91"/>
+    </row>
+    <row r="37" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="70"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="89"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="91"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="57"/>
-    </row>
-    <row r="39" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="77"/>
-      <c r="B39" s="67">
+      <c r="D37" s="65"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="92"/>
+    </row>
+    <row r="38" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="70"/>
+      <c r="B38" s="55">
         <v>18</v>
       </c>
-      <c r="C39" s="79" t="s">
+      <c r="C38" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E38" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F38" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G39" s="51"/>
-      <c r="H39" s="45" t="s">
+      <c r="G38" s="52"/>
+      <c r="H38" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="I39" s="48" t="s">
+      <c r="I38" s="88" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A40" s="77"/>
-      <c r="B40" s="70"/>
-      <c r="C40" s="80"/>
-      <c r="D40" s="19" t="s">
+    <row r="39" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A39" s="70"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="95"/>
+      <c r="D39" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E39" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F39" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="G40" s="52"/>
-      <c r="H40" s="42" t="s">
+      <c r="G39" s="53"/>
+      <c r="H39" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="I40" s="49"/>
-    </row>
-    <row r="41" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="77"/>
-      <c r="B41" s="68"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="22" t="s">
+      <c r="I39" s="89"/>
+    </row>
+    <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="70"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F40" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G41" s="53"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="50"/>
-    </row>
-    <row r="42" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="77"/>
-      <c r="B42" s="35">
+      <c r="G40" s="54"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="90"/>
+    </row>
+    <row r="41" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="70"/>
+      <c r="B41" s="34">
         <v>20</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="15" t="s">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="I42" s="11" t="s">
+      <c r="I41" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="78"/>
-      <c r="B43" s="69" t="s">
+    <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A42" s="51"/>
+      <c r="B42" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="69"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="69"/>
-      <c r="F43" s="69"/>
-      <c r="G43" s="69"/>
-      <c r="H43" s="69"/>
-      <c r="I43" s="87"/>
-    </row>
-    <row r="44" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="78"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="17">
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="63"/>
+    </row>
+    <row r="43" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="51"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="17">
         <v>27</v>
       </c>
-      <c r="D44" s="17">
-        <f t="shared" ref="D44:I44" si="0">COUNTIF(D4:D42, "&lt;&gt;")</f>
+      <c r="D43" s="17">
+        <f t="shared" ref="D43:I43" si="0">COUNTIF(D4:D41, "&lt;&gt;")</f>
         <v>19</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E43" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F44" s="17">
+      <c r="F43" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G44" s="17">
+      <c r="G43" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H44" s="17">
+      <c r="H43" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I44" s="17">
+      <c r="I43" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="78"/>
-      <c r="B45" s="69" t="str">
-        <f>SUM(C44:I44) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
+    <row r="44" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="51"/>
+      <c r="B44" s="62" t="str">
+        <f>SUM(C43:I43) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
         <v>97 Total Races (Prior to Breeders' Cup Weekend)</v>
       </c>
-      <c r="C45" s="69"/>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="69"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="69"/>
-      <c r="I45" s="69"/>
-    </row>
-    <row r="46" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="78"/>
-      <c r="B46" s="82" t="s">
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="62"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="62"/>
+      <c r="I44" s="62"/>
+    </row>
+    <row r="45" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="51"/>
+      <c r="B45" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="C46" s="82"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="83"/>
-      <c r="F46" s="84" t="s">
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="G46" s="85"/>
-      <c r="H46" s="85"/>
-      <c r="I46" s="86"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="80">
+  <mergeCells count="73">
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="A2:A41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="E14:E16"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="B43:I43"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="B34:B37"/>
     <mergeCell ref="C1:I1"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="A2:A42"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="B45:I45"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="I39:I41"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="H35:H38"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="I36:I38"/>
-    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="F14:F16"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RTTR151 Week 4 Noms; RTTBC25 Delaware Park Moves
</commit_message>
<xml_diff>
--- a/pdf/RTTBC25-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC25-Schedule-by-Division.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1166" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE751561-2066-4B69-B288-B084952CB9D3}"/>
+  <xr:revisionPtr revIDLastSave="1182" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39B2CDE8-D381-4582-838F-67336911308D}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="0" windowWidth="27690" windowHeight="20985" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -669,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -816,7 +816,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -827,130 +836,124 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1275,8 +1278,8 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34:F37"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1292,20 +1295,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="51"/>
-      <c r="B1" s="51"/>
-      <c r="C1" s="69" t="s">
+      <c r="A1" s="81"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="80" t="s">
         <v>96</v>
       </c>
       <c r="B2" s="32"/>
@@ -1332,7 +1335,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="70"/>
+      <c r="A3" s="80"/>
       <c r="B3" s="33"/>
       <c r="C3" s="31" t="s">
         <v>5</v>
@@ -1357,8 +1360,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="70"/>
-      <c r="B4" s="55">
+      <c r="A4" s="80"/>
+      <c r="B4" s="71">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1367,53 +1370,55 @@
       <c r="D4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="73" t="s">
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="52"/>
+      <c r="H4" s="55"/>
       <c r="I4" s="9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="68"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="53"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="56"/>
       <c r="I5" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="70"/>
-      <c r="B6" s="56"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="54"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="57"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="70"/>
+      <c r="A7" s="80"/>
       <c r="B7" s="34">
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="97" t="s">
+        <v>15</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="11" t="s">
@@ -1425,7 +1430,7 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="70"/>
+      <c r="A8" s="80"/>
       <c r="B8" s="34">
         <v>3</v>
       </c>
@@ -1441,8 +1446,8 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" s="93" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="70"/>
+    <row r="9" spans="1:9" s="51" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="80"/>
       <c r="B9" s="40">
         <v>4</v>
       </c>
@@ -1461,60 +1466,56 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
-      <c r="B10" s="55">
+      <c r="A10" s="80"/>
+      <c r="B10" s="71">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="76"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="68"/>
       <c r="H10" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="76" t="s">
+      <c r="I10" s="68" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="70"/>
-      <c r="B11" s="68"/>
+      <c r="A11" s="80"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="83"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="83"/>
+      <c r="I11" s="69"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="70"/>
-      <c r="B12" s="68"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="83"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="69"/>
       <c r="H12" s="38"/>
-      <c r="I12" s="83"/>
+      <c r="I12" s="69"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="70"/>
+      <c r="A13" s="80"/>
       <c r="B13" s="34">
         <v>6</v>
       </c>
@@ -1529,8 +1530,8 @@
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="70"/>
-      <c r="B14" s="55">
+      <c r="A14" s="80"/>
+      <c r="B14" s="71">
         <v>7</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1539,157 +1540,157 @@
       <c r="D14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="78" t="s">
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="52"/>
+      <c r="I14" s="55"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="70"/>
-      <c r="B15" s="68"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="19" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="53"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="70"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
       <c r="H16" s="79"/>
-      <c r="I16" s="54"/>
+      <c r="I16" s="57"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="70"/>
-      <c r="B17" s="55">
+      <c r="A17" s="80"/>
+      <c r="B17" s="71">
         <v>8</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="76" t="s">
+      <c r="D17" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
       <c r="I17" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="70"/>
-      <c r="B18" s="68"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="83"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
       <c r="I18" s="10" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="70"/>
-      <c r="B19" s="56"/>
+      <c r="A19" s="80"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
       <c r="I19" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="70"/>
-      <c r="B20" s="55">
+      <c r="A20" s="80"/>
+      <c r="B20" s="71">
         <v>9</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="73" t="s">
+      <c r="D20" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="76" t="s">
+      <c r="E20" s="55"/>
+      <c r="F20" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="71" t="s">
+      <c r="G20" s="55"/>
+      <c r="H20" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="52"/>
+      <c r="I20" s="55"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="70"/>
-      <c r="B21" s="68"/>
+      <c r="A21" s="80"/>
+      <c r="B21" s="74"/>
       <c r="C21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="74"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="53"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="56"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="70"/>
-      <c r="B22" s="55">
+      <c r="A22" s="80"/>
+      <c r="B22" s="71">
         <v>10</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="52"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
       <c r="E22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="76" t="s">
+      <c r="F22" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
+      <c r="A23" s="80"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="77"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="57"/>
     </row>
     <row r="24" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="70"/>
+      <c r="A24" s="80"/>
       <c r="B24" s="40">
         <v>11</v>
       </c>
@@ -1706,96 +1707,96 @@
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="70"/>
-      <c r="B25" s="55">
+      <c r="A25" s="80"/>
+      <c r="B25" s="71">
         <v>12</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="71" t="s">
+      <c r="D25" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="52"/>
-      <c r="F25" s="85"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="65"/>
       <c r="G25" s="23" t="s">
         <v>46</v>
       </c>
       <c r="H25" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I25" s="52"/>
+      <c r="I25" s="55"/>
     </row>
     <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="70"/>
-      <c r="B26" s="68"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="72"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="86"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="66"/>
       <c r="G26" s="21" t="s">
         <v>47</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I26" s="53"/>
+      <c r="I26" s="56"/>
     </row>
     <row r="27" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="70"/>
-      <c r="B27" s="56"/>
+      <c r="A27" s="80"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="87"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="67"/>
       <c r="G27" s="14" t="s">
         <v>50</v>
       </c>
       <c r="H27" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="I27" s="54"/>
+      <c r="I27" s="57"/>
     </row>
     <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="70"/>
-      <c r="B28" s="55">
+      <c r="A28" s="80"/>
+      <c r="B28" s="71">
         <v>13</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="76" t="s">
+      <c r="D28" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="71" t="s">
+      <c r="E28" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="81" t="s">
+      <c r="F28" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="52"/>
-      <c r="H28" s="76" t="s">
+      <c r="G28" s="55"/>
+      <c r="H28" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="I28" s="52"/>
+      <c r="I28" s="55"/>
     </row>
     <row r="29" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="70"/>
-      <c r="B29" s="56"/>
+      <c r="A29" s="80"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="77"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="82"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="77"/>
-      <c r="I29" s="54"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="76"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="57"/>
     </row>
     <row r="30" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="70"/>
+      <c r="A30" s="80"/>
       <c r="B30" s="34">
         <v>14</v>
       </c>
@@ -1812,7 +1813,7 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="70"/>
+      <c r="A31" s="80"/>
       <c r="B31" s="34">
         <v>15</v>
       </c>
@@ -1831,58 +1832,58 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="70"/>
-      <c r="B32" s="55">
+      <c r="A32" s="80"/>
+      <c r="B32" s="71">
         <v>16</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="71" t="s">
+      <c r="D32" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="85"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="52"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="55"/>
+      <c r="G32" s="55"/>
       <c r="H32" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="78" t="s">
+      <c r="I32" s="58" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="70"/>
-      <c r="B33" s="68"/>
+      <c r="A33" s="80"/>
+      <c r="B33" s="74"/>
       <c r="C33" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="72"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
       <c r="H33" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="I33" s="84"/>
+      <c r="I33" s="59"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="70"/>
-      <c r="B34" s="55">
+      <c r="A34" s="80"/>
+      <c r="B34" s="71">
         <v>17</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="64" t="s">
+      <c r="D34" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="66" t="s">
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="78" t="s">
+      <c r="H34" s="58" t="s">
         <v>68</v>
       </c>
       <c r="I34" s="8" t="s">
@@ -1890,52 +1891,54 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="70"/>
-      <c r="B35" s="68"/>
+      <c r="A35" s="80"/>
+      <c r="B35" s="74"/>
       <c r="C35" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="65"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="84"/>
-      <c r="I35" s="91" t="s">
+      <c r="D35" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="60" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="70"/>
-      <c r="B36" s="68"/>
+      <c r="A36" s="80"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="65"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="84"/>
-      <c r="I36" s="91"/>
+      <c r="D36" s="92"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="94"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="60"/>
     </row>
     <row r="37" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="70"/>
-      <c r="B37" s="68"/>
+      <c r="A37" s="80"/>
+      <c r="B37" s="74"/>
       <c r="C37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="65"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="67"/>
-      <c r="H37" s="84"/>
-      <c r="I37" s="92"/>
+      <c r="D37" s="96"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="61"/>
     </row>
     <row r="38" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="70"/>
-      <c r="B38" s="55">
+      <c r="A38" s="80"/>
+      <c r="B38" s="71">
         <v>18</v>
       </c>
-      <c r="C38" s="94" t="s">
+      <c r="C38" s="82" t="s">
         <v>74</v>
       </c>
       <c r="D38" s="6" t="s">
@@ -1947,18 +1950,18 @@
       <c r="F38" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G38" s="52"/>
+      <c r="G38" s="55"/>
       <c r="H38" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="I38" s="88" t="s">
+      <c r="I38" s="52" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A39" s="70"/>
-      <c r="B39" s="68"/>
-      <c r="C39" s="95"/>
+      <c r="A39" s="80"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="83"/>
       <c r="D39" s="19" t="s">
         <v>82</v>
       </c>
@@ -1968,16 +1971,16 @@
       <c r="F39" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="G39" s="53"/>
+      <c r="G39" s="56"/>
       <c r="H39" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="I39" s="89"/>
+      <c r="I39" s="53"/>
     </row>
     <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="70"/>
-      <c r="B40" s="56"/>
-      <c r="C40" s="96"/>
+      <c r="A40" s="80"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="84"/>
       <c r="D40" s="3"/>
       <c r="E40" s="22" t="s">
         <v>80</v>
@@ -1985,12 +1988,12 @@
       <c r="F40" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G40" s="54"/>
+      <c r="G40" s="57"/>
       <c r="H40" s="45"/>
-      <c r="I40" s="90"/>
+      <c r="I40" s="54"/>
     </row>
     <row r="41" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="70"/>
+      <c r="A41" s="80"/>
       <c r="B41" s="34">
         <v>20</v>
       </c>
@@ -2007,20 +2010,20 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A42" s="51"/>
-      <c r="B42" s="62" t="s">
+      <c r="A42" s="81"/>
+      <c r="B42" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="62"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="63"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="91"/>
     </row>
     <row r="43" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="51"/>
+      <c r="A43" s="81"/>
       <c r="B43" s="18"/>
       <c r="C43" s="17">
         <v>27</v>
@@ -2051,68 +2054,63 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="51"/>
-      <c r="B44" s="62" t="str">
+      <c r="A44" s="81"/>
+      <c r="B44" s="73" t="str">
         <f>SUM(C43:I43) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
         <v>97 Total Races (Prior to Breeders' Cup Weekend)</v>
       </c>
-      <c r="C44" s="62"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="62"/>
-      <c r="F44" s="62"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="62"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73"/>
+      <c r="I44" s="73"/>
     </row>
     <row r="45" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="51"/>
-      <c r="B45" s="57" t="s">
+      <c r="A45" s="81"/>
+      <c r="B45" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="58"/>
-      <c r="F45" s="59" t="s">
+      <c r="C45" s="86"/>
+      <c r="D45" s="86"/>
+      <c r="E45" s="87"/>
+      <c r="F45" s="88" t="s">
         <v>93</v>
       </c>
-      <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="61"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="89"/>
+      <c r="I45" s="90"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="I35:I37"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
+  <mergeCells count="74">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="E34:E37"/>
+    <mergeCell ref="F34:F37"/>
+    <mergeCell ref="G34:G37"/>
+    <mergeCell ref="B34:B37"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A2:A41"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="D10:D12"/>
     <mergeCell ref="B44:I44"/>
     <mergeCell ref="G38:G40"/>
     <mergeCell ref="B4:B6"/>
@@ -2128,32 +2126,38 @@
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="H14:H16"/>
-    <mergeCell ref="A2:A41"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="D34:D37"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="I22:I23"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GRCW-900; Other OFF TRAIL Updates; GRCW-902; GRCW-901 (partial)
</commit_message>
<xml_diff>
--- a/pdf/RTTBC25-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC25-Schedule-by-Division.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1182" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39B2CDE8-D381-4582-838F-67336911308D}"/>
+  <xr:revisionPtr revIDLastSave="1231" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5BA328C-6475-48A5-A278-BA95AC78BCDB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
@@ -387,7 +387,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,6 +504,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -669,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -736,9 +744,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -812,20 +817,17 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -836,77 +838,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -917,44 +895,83 @@
     <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1278,13 +1295,13 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14:F16"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38:I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="34" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -1295,73 +1312,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="81"/>
-      <c r="B1" s="81"/>
-      <c r="C1" s="95" t="s">
+      <c r="A1" s="52"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="29" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="80"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="31" t="s">
+      <c r="A3" s="70"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="80"/>
-      <c r="B4" s="71">
+      <c r="A4" s="70"/>
+      <c r="B4" s="65">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1370,53 +1387,53 @@
       <c r="D4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
       <c r="G4" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="55"/>
+      <c r="H4" s="53"/>
       <c r="I4" s="9" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="80"/>
-      <c r="B5" s="74"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
       <c r="G5" s="78"/>
-      <c r="H5" s="56"/>
+      <c r="H5" s="54"/>
       <c r="I5" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="80"/>
-      <c r="B6" s="72"/>
+      <c r="A6" s="70"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="57"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="55"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="80"/>
-      <c r="B7" s="34">
+      <c r="A7" s="70"/>
+      <c r="B7" s="33">
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="51" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="4"/>
@@ -1430,8 +1447,8 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="80"/>
-      <c r="B8" s="34">
+      <c r="A8" s="70"/>
+      <c r="B8" s="33">
         <v>3</v>
       </c>
       <c r="C8" s="11" t="s">
@@ -1441,82 +1458,82 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="93" t="s">
         <v>108</v>
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" s="51" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="80"/>
-      <c r="B9" s="40">
+    <row r="9" spans="1:9" s="49" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="70"/>
+      <c r="B9" s="39">
         <v>4</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="48" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="37" t="s">
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="36" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="80"/>
-      <c r="B10" s="71">
+      <c r="A10" s="70"/>
+      <c r="B10" s="65">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="37" t="s">
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="68" t="s">
+      <c r="I10" s="80" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="80"/>
-      <c r="B11" s="74"/>
+      <c r="A11" s="70"/>
+      <c r="B11" s="66"/>
       <c r="C11" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="69"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="39" t="s">
+      <c r="D11" s="82"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="69"/>
+      <c r="I11" s="82"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="80"/>
-      <c r="B12" s="74"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="66"/>
       <c r="C12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="70"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="69"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="82"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="80"/>
-      <c r="B13" s="34">
+      <c r="A13" s="70"/>
+      <c r="B13" s="33">
         <v>6</v>
       </c>
       <c r="C13" s="4"/>
@@ -1530,8 +1547,8 @@
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="80"/>
-      <c r="B14" s="71">
+      <c r="A14" s="70"/>
+      <c r="B14" s="65">
         <v>7</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1540,94 +1557,94 @@
       <c r="D14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="58" t="s">
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="55"/>
+      <c r="I14" s="53"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="80"/>
-      <c r="B15" s="74"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="19" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="56"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="54"/>
+      <c r="G15" s="54"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="54"/>
     </row>
     <row r="16" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="80"/>
-      <c r="B16" s="72"/>
+      <c r="A16" s="70"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="57"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="55"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="80"/>
-      <c r="B17" s="71">
+      <c r="A17" s="70"/>
+      <c r="B17" s="65">
         <v>8</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="68" t="s">
+      <c r="D17" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="53"/>
       <c r="I17" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="80"/>
-      <c r="B18" s="74"/>
-      <c r="C18" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="69"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="56"/>
-      <c r="H18" s="56"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="54"/>
       <c r="I18" s="10" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="80"/>
-      <c r="B19" s="72"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="55"/>
       <c r="I19" s="22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="80"/>
-      <c r="B20" s="71">
+      <c r="A20" s="70"/>
+      <c r="B20" s="65">
         <v>9</v>
       </c>
       <c r="C20" s="20" t="s">
@@ -1636,176 +1653,176 @@
       <c r="D20" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="55"/>
-      <c r="F20" s="68" t="s">
+      <c r="E20" s="53"/>
+      <c r="F20" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="55"/>
-      <c r="H20" s="62" t="s">
+      <c r="G20" s="53"/>
+      <c r="H20" s="75" t="s">
         <v>103</v>
       </c>
-      <c r="I20" s="55"/>
+      <c r="I20" s="53"/>
     </row>
     <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="80"/>
-      <c r="B21" s="74"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="66"/>
       <c r="C21" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="78"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="63"/>
-      <c r="I21" s="56"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="82"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="80"/>
-      <c r="B22" s="71">
+      <c r="A22" s="70"/>
+      <c r="B22" s="65">
         <v>10</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
       <c r="E22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="68" t="s">
+      <c r="F22" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
     </row>
     <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="80"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
+      <c r="A23" s="70"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
       <c r="E23" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="70"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
     </row>
     <row r="24" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="80"/>
-      <c r="B24" s="40">
+      <c r="A24" s="70"/>
+      <c r="B24" s="39">
         <v>11</v>
       </c>
-      <c r="C24" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="36" t="s">
+      <c r="C24" s="42"/>
+      <c r="D24" s="35" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="42" t="s">
+        <v>43</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="80"/>
-      <c r="B25" s="71">
+      <c r="A25" s="70"/>
+      <c r="B25" s="65">
         <v>12</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="62" t="s">
+      <c r="D25" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="55"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="23" t="s">
+      <c r="E25" s="53"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H25" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I25" s="55"/>
+      <c r="I25" s="53"/>
     </row>
     <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="80"/>
-      <c r="B26" s="74"/>
+      <c r="A26" s="70"/>
+      <c r="B26" s="66"/>
       <c r="C26" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="63"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="66"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="88"/>
       <c r="G26" s="21" t="s">
         <v>47</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I26" s="56"/>
+      <c r="I26" s="54"/>
     </row>
     <row r="27" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="80"/>
-      <c r="B27" s="72"/>
+      <c r="A27" s="70"/>
+      <c r="B27" s="71"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="67"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="89"/>
       <c r="G27" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="H27" s="25" t="s">
+      <c r="H27" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="I27" s="57"/>
+      <c r="I27" s="55"/>
     </row>
     <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="80"/>
-      <c r="B28" s="71">
+      <c r="A28" s="70"/>
+      <c r="B28" s="65">
         <v>13</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="68" t="s">
+      <c r="D28" s="80" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="62" t="s">
+      <c r="E28" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="75" t="s">
+      <c r="F28" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="55"/>
-      <c r="H28" s="68" t="s">
+      <c r="G28" s="53"/>
+      <c r="H28" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="I28" s="55"/>
+      <c r="I28" s="53"/>
     </row>
     <row r="29" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="80"/>
-      <c r="B29" s="72"/>
+      <c r="A29" s="70"/>
+      <c r="B29" s="71"/>
       <c r="C29" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="70"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="57"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="83"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="55"/>
     </row>
     <row r="30" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="80"/>
-      <c r="B30" s="34">
+      <c r="A30" s="70"/>
+      <c r="B30" s="33">
         <v>14</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="27" t="s">
+      <c r="F30" s="26" t="s">
         <v>56</v>
       </c>
       <c r="G30" s="5"/>
@@ -1813,18 +1830,18 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="80"/>
-      <c r="B31" s="34">
+      <c r="A31" s="70"/>
+      <c r="B31" s="33">
         <v>15</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="F31" s="28" t="s">
         <v>59</v>
       </c>
       <c r="G31" s="5"/>
@@ -1832,44 +1849,44 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="80"/>
-      <c r="B32" s="71">
+      <c r="A32" s="70"/>
+      <c r="B32" s="65">
         <v>16</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="62" t="s">
+      <c r="D32" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="E32" s="65"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="37" t="s">
+      <c r="E32" s="87"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="58" t="s">
+      <c r="I32" s="84" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="80"/>
-      <c r="B33" s="74"/>
+      <c r="A33" s="70"/>
+      <c r="B33" s="66"/>
       <c r="C33" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D33" s="63"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="56"/>
-      <c r="G33" s="56"/>
-      <c r="H33" s="42" t="s">
+      <c r="D33" s="76"/>
+      <c r="E33" s="88"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="I33" s="59"/>
+      <c r="I33" s="85"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="80"/>
-      <c r="B34" s="71">
+      <c r="A34" s="70"/>
+      <c r="B34" s="65">
         <v>17</v>
       </c>
       <c r="C34" s="6" t="s">
@@ -1878,12 +1895,12 @@
       <c r="D34" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="93" t="s">
+      <c r="E34" s="53"/>
+      <c r="F34" s="53"/>
+      <c r="G34" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="H34" s="58" t="s">
+      <c r="H34" s="84" t="s">
         <v>68</v>
       </c>
       <c r="I34" s="8" t="s">
@@ -1891,57 +1908,57 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="80"/>
-      <c r="B35" s="74"/>
+      <c r="A35" s="70"/>
+      <c r="B35" s="66"/>
       <c r="C35" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="94" t="s">
         <v>111</v>
       </c>
-      <c r="E35" s="56"/>
-      <c r="F35" s="56"/>
-      <c r="G35" s="94"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="60" t="s">
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="100" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="80"/>
-      <c r="B36" s="74"/>
-      <c r="C36" s="46" t="s">
+      <c r="A36" s="70"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="D36" s="92"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="94"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="60"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="96"/>
     </row>
     <row r="37" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="80"/>
-      <c r="B37" s="74"/>
+      <c r="A37" s="70"/>
+      <c r="B37" s="66"/>
       <c r="C37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="96"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="94"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="61"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="85"/>
+      <c r="I37" s="97"/>
     </row>
     <row r="38" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="80"/>
-      <c r="B38" s="71">
+      <c r="A38" s="70"/>
+      <c r="B38" s="65">
         <v>18</v>
       </c>
-      <c r="C38" s="82" t="s">
+      <c r="C38" s="72" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="95" t="s">
         <v>81</v>
       </c>
       <c r="E38" s="20" t="s">
@@ -1950,37 +1967,37 @@
       <c r="F38" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G38" s="55"/>
-      <c r="H38" s="44" t="s">
+      <c r="G38" s="53"/>
+      <c r="H38" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="I38" s="52" t="s">
+      <c r="I38" s="90" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A39" s="80"/>
-      <c r="B39" s="74"/>
-      <c r="C39" s="83"/>
+      <c r="A39" s="70"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="73"/>
       <c r="D39" s="19" t="s">
         <v>82</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="G39" s="56"/>
-      <c r="H39" s="41" t="s">
+      <c r="G39" s="54"/>
+      <c r="H39" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="I39" s="53"/>
+      <c r="I39" s="91"/>
     </row>
     <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="80"/>
-      <c r="B40" s="72"/>
-      <c r="C40" s="84"/>
+      <c r="A40" s="70"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="74"/>
       <c r="D40" s="3"/>
       <c r="E40" s="22" t="s">
         <v>80</v>
@@ -1988,13 +2005,13 @@
       <c r="F40" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="G40" s="57"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="54"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="92"/>
     </row>
     <row r="41" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="80"/>
-      <c r="B41" s="34">
+      <c r="A41" s="70"/>
+      <c r="B41" s="33">
         <v>20</v>
       </c>
       <c r="C41" s="5"/>
@@ -2010,20 +2027,20 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A42" s="81"/>
-      <c r="B42" s="73" t="s">
+      <c r="A42" s="52"/>
+      <c r="B42" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
-      <c r="F42" s="73"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="91"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="62"/>
     </row>
     <row r="43" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="81"/>
+      <c r="A43" s="52"/>
       <c r="B43" s="18"/>
       <c r="C43" s="17">
         <v>27</v>
@@ -2042,7 +2059,7 @@
       </c>
       <c r="G43" s="17">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H43" s="17">
         <f t="shared" si="0"/>
@@ -2054,36 +2071,95 @@
       </c>
     </row>
     <row r="44" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="81"/>
-      <c r="B44" s="73" t="str">
+      <c r="A44" s="52"/>
+      <c r="B44" s="61" t="str">
         <f>SUM(C43:I43) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
-        <v>97 Total Races (Prior to Breeders' Cup Weekend)</v>
-      </c>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="73"/>
-      <c r="I44" s="73"/>
+        <v>99 Total Races (Prior to Breeders' Cup Weekend)</v>
+      </c>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="61"/>
     </row>
     <row r="45" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="81"/>
-      <c r="B45" s="86" t="s">
+      <c r="A45" s="52"/>
+      <c r="B45" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="86"/>
-      <c r="D45" s="86"/>
-      <c r="E45" s="87"/>
-      <c r="F45" s="88" t="s">
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="G45" s="89"/>
-      <c r="H45" s="89"/>
-      <c r="I45" s="90"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="74">
+  <mergeCells count="75">
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="H34:H37"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="B44:I44"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="E10:E12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="F4:F6"/>
@@ -2100,64 +2176,6 @@
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="A2:A41"/>
     <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="I35:I37"/>
-    <mergeCell ref="I22:I23"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GRCW-892, 889, 885, 890
</commit_message>
<xml_diff>
--- a/pdf/RTTBC25-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC25-Schedule-by-Division.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1231" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5BA328C-6475-48A5-A278-BA95AC78BCDB}"/>
+  <xr:revisionPtr revIDLastSave="1244" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F55AF760-2AE1-46E9-8DC7-A9F3635AB107}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="113">
   <si>
     <t>9 Furlongs</t>
   </si>
@@ -335,9 +335,6 @@
     <t>Princess Rooney Invt'l-G3</t>
   </si>
   <si>
-    <t>Brooklyn S-G2</t>
-  </si>
-  <si>
     <t>Travers S.-G1</t>
   </si>
   <si>
@@ -375,9 +372,6 @@
   </si>
   <si>
     <t>Alfred G. Vanderbilt H.-G2</t>
-  </si>
-  <si>
-    <t>John A. Nerud S.-G3</t>
   </si>
   <si>
     <t>True North H.-G3</t>
@@ -677,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -781,9 +775,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -826,18 +817,123 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -853,9 +949,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -865,113 +958,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -993,6 +984,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1292,11 +1287,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1783450-6415-4D0D-A0B8-DEE615502A89}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I38" sqref="I38:I40"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1312,20 +1307,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="52"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="67" t="s">
+      <c r="A1" s="89"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="98" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="99" t="s">
         <v>96</v>
       </c>
       <c r="B2" s="31"/>
@@ -1352,7 +1347,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="70"/>
+      <c r="A3" s="99"/>
       <c r="B3" s="32"/>
       <c r="C3" s="30" t="s">
         <v>5</v>
@@ -1377,8 +1372,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="70"/>
-      <c r="B4" s="65">
+      <c r="A4" s="99"/>
+      <c r="B4" s="79">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1387,53 +1382,53 @@
       <c r="D4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="77" t="s">
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="64"/>
       <c r="I4" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="70"/>
-      <c r="B5" s="66"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="54"/>
+        <v>109</v>
+      </c>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="65"/>
       <c r="I5" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="70"/>
-      <c r="B6" s="71"/>
+      <c r="A6" s="99"/>
+      <c r="B6" s="81"/>
       <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="55"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="66"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="70"/>
+      <c r="A7" s="99"/>
       <c r="B7" s="33">
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="50" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="4"/>
@@ -1447,7 +1442,7 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="70"/>
+      <c r="A8" s="99"/>
       <c r="B8" s="33">
         <v>3</v>
       </c>
@@ -1458,724 +1453,698 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="93" t="s">
+      <c r="H8" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" s="48" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="99"/>
+      <c r="B9" s="38">
+        <v>4</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" s="49" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="70"/>
-      <c r="B9" s="39">
-        <v>4</v>
-      </c>
-      <c r="C9" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="36" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
-      <c r="B10" s="65">
+      <c r="A10" s="99"/>
+      <c r="B10" s="79">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="80" t="s">
+      <c r="D10" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="80"/>
+      <c r="E10" s="73" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="64"/>
+      <c r="G10" s="76"/>
       <c r="H10" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="80" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="70"/>
-      <c r="B11" s="66"/>
+      <c r="I10" s="76"/>
+    </row>
+    <row r="11" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="99"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="77"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="77"/>
+    </row>
+    <row r="12" spans="1:9" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="99"/>
+      <c r="B12" s="33">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="99"/>
+      <c r="B13" s="79">
+        <v>7</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="99"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+    </row>
+    <row r="15" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="99"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="99"/>
+      <c r="B16" s="79">
+        <v>8</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="64"/>
+      <c r="I16" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="99"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="84"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="99"/>
+      <c r="B18" s="79">
+        <v>9</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="70" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="64"/>
+      <c r="F18" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="64"/>
+      <c r="H18" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" s="64"/>
+    </row>
+    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="99"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="71"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="65"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="99"/>
+      <c r="B20" s="79">
+        <v>10</v>
+      </c>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+    </row>
+    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="99"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="84"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+    </row>
+    <row r="22" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="99"/>
+      <c r="B22" s="38">
+        <v>11</v>
+      </c>
+      <c r="C22" s="41"/>
+      <c r="D22" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A23" s="99"/>
+      <c r="B23" s="79">
+        <v>12</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="64"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="64"/>
+    </row>
+    <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="99"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="82"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="38" t="s">
+      <c r="D24" s="71"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="65"/>
+    </row>
+    <row r="25" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="99"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25" s="66"/>
+    </row>
+    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A26" s="99"/>
+      <c r="B26" s="79">
+        <v>13</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="82" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="64"/>
+      <c r="H26" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" s="64"/>
+    </row>
+    <row r="27" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="99"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="84"/>
+      <c r="E27" s="83"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="66"/>
+    </row>
+    <row r="28" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="99"/>
+      <c r="B28" s="33">
+        <v>14</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="99"/>
+      <c r="B29" s="33">
+        <v>15</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="99"/>
+      <c r="B30" s="79">
         <v>16</v>
       </c>
-      <c r="I11" s="82"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="70"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="82"/>
-    </row>
-    <row r="13" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="70"/>
-      <c r="B13" s="33">
-        <v>6</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="70"/>
-      <c r="B14" s="65">
-        <v>7</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="84" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="53"/>
-    </row>
-    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="70"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="85"/>
-      <c r="I15" s="54"/>
-    </row>
-    <row r="16" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="70"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="24" t="s">
+      <c r="C30" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="82" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="73"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="56" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="99"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="88"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="I31" s="57"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="99"/>
+      <c r="B32" s="79">
+        <v>17</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A33" s="99"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="57"/>
+      <c r="I33" s="55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="99"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="68"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="57"/>
+      <c r="I34" s="59"/>
+    </row>
+    <row r="35" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="99"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="69"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="60"/>
+    </row>
+    <row r="36" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="99"/>
+      <c r="B36" s="79">
+        <v>18</v>
+      </c>
+      <c r="C36" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="64"/>
+      <c r="H36" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" s="61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A37" s="99"/>
+      <c r="B37" s="80"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="G37" s="65"/>
+      <c r="H37" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="I37" s="62"/>
+    </row>
+    <row r="38" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="99"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G38" s="66"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="63"/>
+    </row>
+    <row r="39" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="99"/>
+      <c r="B39" s="33">
+        <v>20</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A40" s="89"/>
+      <c r="B40" s="78" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="78"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="78"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="95"/>
+    </row>
+    <row r="41" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="89"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="17">
         <v>27</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="55"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="70"/>
-      <c r="B17" s="65">
-        <v>8</v>
-      </c>
-      <c r="C17" s="84" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="98" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="53"/>
-      <c r="I17" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="70"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="70"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A20" s="70"/>
-      <c r="B20" s="65">
-        <v>9</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="77" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="53"/>
-      <c r="F20" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="53"/>
-      <c r="H20" s="75" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="53"/>
-    </row>
-    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="70"/>
-      <c r="B21" s="66"/>
-      <c r="C21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="78"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="54"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="70"/>
-      <c r="B22" s="65">
-        <v>10</v>
-      </c>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="80" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-    </row>
-    <row r="23" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="70"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="81"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-    </row>
-    <row r="24" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="70"/>
-      <c r="B24" s="39">
-        <v>11</v>
-      </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A25" s="70"/>
-      <c r="B25" s="65">
-        <v>12</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="53"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="H25" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I25" s="53"/>
-    </row>
-    <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="70"/>
-      <c r="B26" s="66"/>
-      <c r="C26" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="78"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H26" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26" s="54"/>
-    </row>
-    <row r="27" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="70"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="I27" s="55"/>
-    </row>
-    <row r="28" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="70"/>
-      <c r="B28" s="65">
-        <v>13</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="75" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="77" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="53"/>
-      <c r="H28" s="80" t="s">
-        <v>105</v>
-      </c>
-      <c r="I28" s="53"/>
-    </row>
-    <row r="29" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="70"/>
-      <c r="B29" s="71"/>
-      <c r="C29" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="81"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="55"/>
-    </row>
-    <row r="30" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="70"/>
-      <c r="B30" s="33">
-        <v>14</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="70"/>
-      <c r="B31" s="33">
-        <v>15</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A32" s="70"/>
-      <c r="B32" s="65">
-        <v>16</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="87"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" s="84" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="70"/>
-      <c r="B33" s="66"/>
-      <c r="C33" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="76"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="I33" s="85"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="70"/>
-      <c r="B34" s="65">
-        <v>17</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D34" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="63" t="s">
-        <v>72</v>
-      </c>
-      <c r="H34" s="84" t="s">
-        <v>68</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="70"/>
-      <c r="B35" s="66"/>
-      <c r="C35" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="94" t="s">
-        <v>111</v>
-      </c>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="85"/>
-      <c r="I35" s="100" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="70"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="68"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="85"/>
-      <c r="I36" s="96"/>
-    </row>
-    <row r="37" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="70"/>
-      <c r="B37" s="66"/>
-      <c r="C37" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" s="69"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="85"/>
-      <c r="I37" s="97"/>
-    </row>
-    <row r="38" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="70"/>
-      <c r="B38" s="65">
-        <v>18</v>
-      </c>
-      <c r="C38" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="95" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" s="53"/>
-      <c r="H38" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="I38" s="90" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A39" s="70"/>
-      <c r="B39" s="66"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F39" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="G39" s="54"/>
-      <c r="H39" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="I39" s="91"/>
-    </row>
-    <row r="40" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="70"/>
-      <c r="B40" s="71"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="G40" s="55"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="92"/>
-    </row>
-    <row r="41" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="70"/>
-      <c r="B41" s="33">
-        <v>20</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A42" s="52"/>
-      <c r="B42" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="61"/>
-      <c r="I42" s="62"/>
-    </row>
-    <row r="43" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="52"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="17">
-        <v>27</v>
-      </c>
-      <c r="D43" s="17">
-        <f t="shared" ref="D43:I43" si="0">COUNTIF(D4:D41, "&lt;&gt;")</f>
+      <c r="D41" s="17">
+        <f t="shared" ref="D41:I41" si="0">COUNTIF(D4:D39, "&lt;&gt;")</f>
         <v>19</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E41" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F43" s="17">
+      <c r="F41" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G43" s="17">
+      <c r="G41" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="H43" s="17">
+      <c r="H41" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="I43" s="17">
+      <c r="I41" s="17">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="52"/>
-      <c r="B44" s="61" t="str">
-        <f>SUM(C43:I43) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
-        <v>99 Total Races (Prior to Breeders' Cup Weekend)</v>
-      </c>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="61"/>
-    </row>
-    <row r="45" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="52"/>
-      <c r="B45" s="56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="89"/>
+      <c r="B42" s="78" t="str">
+        <f>SUM(C41:I41) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
+        <v>98 Total Races (Prior to Breeders' Cup Weekend)</v>
+      </c>
+      <c r="C42" s="78"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="78"/>
+      <c r="H42" s="78"/>
+      <c r="I42" s="78"/>
+    </row>
+    <row r="43" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="89"/>
+      <c r="B43" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="58" t="s">
+      <c r="C43" s="90"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="91"/>
+      <c r="F43" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="G45" s="59"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="60"/>
+      <c r="G43" s="93"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="H34:H37"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="B44:I44"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="G32:G35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A2:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C20:C21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="F20:F21"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G20:G21"/>
     <mergeCell ref="H20:H21"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="E34:E37"/>
-    <mergeCell ref="F34:F37"/>
-    <mergeCell ref="G34:G37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A2:A41"/>
-    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I36:I38"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="H32:H35"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="G30:G31"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GRCW-908, 886, 887, 891, 888, 859
</commit_message>
<xml_diff>
--- a/pdf/RTTBC25-Schedule-by-Division.xlsx
+++ b/pdf/RTTBC25-Schedule-by-Division.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/pdf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1244" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F55AF760-2AE1-46E9-8DC7-A9F3635AB107}"/>
+  <xr:revisionPtr revIDLastSave="1278" documentId="8_{DAECCBE5-FF72-4188-B2F1-1541968A3FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9E25E3E-2A50-4B04-A6F9-69F9662E656B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EAD27B02-19FE-4D48-9014-ED6E24DB84F0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
   <si>
     <t>9 Furlongs</t>
   </si>
@@ -375,13 +375,16 @@
   </si>
   <si>
     <t>True North H.-G3</t>
+  </si>
+  <si>
+    <t>Acorn S.-G1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +509,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -671,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -832,6 +841,108 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -839,6 +950,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -856,113 +970,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1290,8 +1302,8 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18:I19"/>
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1307,20 +1319,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="89"/>
-      <c r="B1" s="89"/>
-      <c r="C1" s="98" t="s">
+      <c r="A1" s="56"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="74" t="s">
         <v>96</v>
       </c>
       <c r="B2" s="31"/>
@@ -1347,7 +1359,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="99"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="32"/>
       <c r="C3" s="30" t="s">
         <v>5</v>
@@ -1372,8 +1384,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="99"/>
-      <c r="B4" s="79">
+      <c r="A4" s="74"/>
+      <c r="B4" s="69">
         <v>1</v>
       </c>
       <c r="C4" s="23" t="s">
@@ -1382,48 +1394,50 @@
       <c r="D4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="70" t="s">
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="64"/>
+      <c r="H4" s="90" t="s">
+        <v>97</v>
+      </c>
       <c r="I4" s="9" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="99"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="65"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="100" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="91"/>
       <c r="I5" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="99"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="3"/>
+    <row r="6" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="74"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="99"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="33">
         <v>2</v>
       </c>
@@ -1436,13 +1450,11 @@
       <c r="G7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>97</v>
-      </c>
+      <c r="H7" s="15"/>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="99"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="33">
         <v>3</v>
       </c>
@@ -1459,7 +1471,7 @@
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" s="48" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="38">
         <v>4</v>
       </c>
@@ -1478,205 +1490,207 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
-      <c r="B10" s="79">
+      <c r="A10" s="74"/>
+      <c r="B10" s="69">
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="76" t="s">
+      <c r="D10" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="76"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="84"/>
       <c r="H10" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="76"/>
-    </row>
-    <row r="11" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="99"/>
-      <c r="B11" s="80"/>
+      <c r="I10" s="84"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="74"/>
+      <c r="B11" s="70"/>
       <c r="C11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="77"/>
+        <v>18</v>
+      </c>
+      <c r="D11" s="86"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="86"/>
       <c r="H11" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="77"/>
-    </row>
-    <row r="12" spans="1:9" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="99"/>
-      <c r="B12" s="33">
+      <c r="I11" s="86"/>
+    </row>
+    <row r="12" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="74"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="86"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="86"/>
+    </row>
+    <row r="13" spans="1:9" ht="19.5" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="74"/>
+      <c r="B13" s="33">
         <v>6</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A13" s="99"/>
-      <c r="B13" s="79">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="74"/>
+      <c r="B14" s="69">
         <v>7</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="56" t="s">
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="I13" s="56" t="s">
+      <c r="I14" s="90" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A14" s="99"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="19" t="s">
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="74"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-    </row>
-    <row r="15" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="99"/>
-      <c r="B15" s="81"/>
-      <c r="C15" s="12" t="s">
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+    </row>
+    <row r="16" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="74"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="99"/>
-      <c r="B16" s="79">
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="74"/>
+      <c r="B17" s="69">
         <v>8</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C17" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="76" t="s">
+      <c r="D17" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="67" t="s">
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="64"/>
-      <c r="I16" s="6" t="s">
+      <c r="H17" s="57"/>
+      <c r="I17" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="99"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="22" t="s">
+    <row r="18" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="74"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="99"/>
-      <c r="B18" s="79">
+    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="A19" s="74"/>
+      <c r="B19" s="69">
         <v>9</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C19" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="70" t="s">
+      <c r="D19" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="64"/>
-      <c r="F18" s="76" t="s">
+      <c r="E19" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="64"/>
-      <c r="H18" s="82" t="s">
+      <c r="G19" s="57"/>
+      <c r="H19" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="64"/>
-    </row>
-    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="99"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="7" t="s">
+      <c r="I19" s="57"/>
+    </row>
+    <row r="20" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="74"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="71"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="65"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="99"/>
-      <c r="B20" s="79">
+      <c r="D20" s="82"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="58"/>
+    </row>
+    <row r="21" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="74"/>
+      <c r="B21" s="38">
         <v>10</v>
       </c>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="76" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-    </row>
-    <row r="21" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="99"/>
-      <c r="B21" s="81"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="84"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="99"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="38">
         <v>11</v>
       </c>
@@ -1693,96 +1707,96 @@
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="99"/>
-      <c r="B23" s="79">
+      <c r="A23" s="74"/>
+      <c r="B23" s="69">
         <v>12</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="70" t="s">
+      <c r="D23" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="64"/>
-      <c r="F23" s="73"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="87"/>
       <c r="G23" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H23" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I23" s="64"/>
+      <c r="I23" s="57"/>
     </row>
     <row r="24" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A24" s="99"/>
-      <c r="B24" s="80"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="70"/>
       <c r="C24" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="71"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="74"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="88"/>
       <c r="G24" s="21" t="s">
         <v>47</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I24" s="65"/>
+      <c r="I24" s="58"/>
     </row>
     <row r="25" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="99"/>
-      <c r="B25" s="81"/>
+      <c r="A25" s="74"/>
+      <c r="B25" s="75"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="75"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="93"/>
       <c r="G25" s="14" t="s">
         <v>50</v>
       </c>
       <c r="H25" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="I25" s="66"/>
+      <c r="I25" s="59"/>
     </row>
     <row r="26" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="99"/>
-      <c r="B26" s="79">
+      <c r="A26" s="74"/>
+      <c r="B26" s="69">
         <v>13</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="76" t="s">
+      <c r="D26" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="82" t="s">
+      <c r="E26" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="F26" s="70" t="s">
+      <c r="F26" s="81" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="64"/>
-      <c r="H26" s="76" t="s">
+      <c r="G26" s="57"/>
+      <c r="H26" s="84" t="s">
         <v>104</v>
       </c>
-      <c r="I26" s="64"/>
+      <c r="I26" s="57"/>
     </row>
     <row r="27" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="99"/>
-      <c r="B27" s="81"/>
+      <c r="A27" s="74"/>
+      <c r="B27" s="75"/>
       <c r="C27" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="84"/>
-      <c r="E27" s="83"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="66"/>
+      <c r="D27" s="85"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="59"/>
     </row>
     <row r="28" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="99"/>
+      <c r="A28" s="74"/>
       <c r="B28" s="33">
         <v>14</v>
       </c>
@@ -1799,7 +1813,7 @@
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="99"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="33">
         <v>15</v>
       </c>
@@ -1818,44 +1832,44 @@
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="99"/>
-      <c r="B30" s="79">
+      <c r="A30" s="74"/>
+      <c r="B30" s="69">
         <v>16</v>
       </c>
       <c r="C30" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="82" t="s">
+      <c r="D30" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="73"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
       <c r="H30" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="I30" s="56" t="s">
+      <c r="I30" s="90" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="99"/>
-      <c r="B31" s="80"/>
+      <c r="A31" s="74"/>
+      <c r="B31" s="70"/>
       <c r="C31" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="88"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="88"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
       <c r="H31" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I31" s="57"/>
+      <c r="I31" s="91"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="99"/>
-      <c r="B32" s="79">
+      <c r="A32" s="74"/>
+      <c r="B32" s="69">
         <v>17</v>
       </c>
       <c r="C32" s="6" t="s">
@@ -1864,12 +1878,12 @@
       <c r="D32" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="96" t="s">
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="H32" s="56" t="s">
+      <c r="H32" s="90" t="s">
         <v>68</v>
       </c>
       <c r="I32" s="8" t="s">
@@ -1877,54 +1891,54 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A33" s="99"/>
-      <c r="B33" s="80"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="70"/>
       <c r="C33" s="19" t="s">
         <v>101</v>
       </c>
       <c r="D33" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="97"/>
-      <c r="H33" s="57"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="91"/>
       <c r="I33" s="55" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="99"/>
-      <c r="B34" s="80"/>
+      <c r="A34" s="74"/>
+      <c r="B34" s="70"/>
       <c r="C34" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="68"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="97"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="59"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="58"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="91"/>
+      <c r="I34" s="94"/>
     </row>
     <row r="35" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="99"/>
-      <c r="B35" s="80"/>
+      <c r="A35" s="74"/>
+      <c r="B35" s="70"/>
       <c r="C35" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="69"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="60"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="91"/>
+      <c r="I35" s="95"/>
     </row>
     <row r="36" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="99"/>
-      <c r="B36" s="79">
+      <c r="A36" s="74"/>
+      <c r="B36" s="69">
         <v>18</v>
       </c>
-      <c r="C36" s="85" t="s">
+      <c r="C36" s="76" t="s">
         <v>74</v>
       </c>
       <c r="D36" s="53" t="s">
@@ -1936,18 +1950,18 @@
       <c r="F36" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G36" s="64"/>
+      <c r="G36" s="57"/>
       <c r="H36" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="I36" s="61" t="s">
+      <c r="I36" s="96" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A37" s="99"/>
-      <c r="B37" s="80"/>
-      <c r="C37" s="86"/>
+      <c r="A37" s="74"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="77"/>
       <c r="D37" s="19" t="s">
         <v>82</v>
       </c>
@@ -1957,16 +1971,16 @@
       <c r="F37" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="65"/>
+      <c r="G37" s="58"/>
       <c r="H37" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="I37" s="62"/>
+      <c r="I37" s="97"/>
     </row>
     <row r="38" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="99"/>
-      <c r="B38" s="81"/>
-      <c r="C38" s="87"/>
+      <c r="A38" s="74"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="3"/>
       <c r="E38" s="22" t="s">
         <v>80</v>
@@ -1974,12 +1988,12 @@
       <c r="F38" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G38" s="66"/>
+      <c r="G38" s="59"/>
       <c r="H38" s="43"/>
-      <c r="I38" s="63"/>
+      <c r="I38" s="98"/>
     </row>
     <row r="39" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="99"/>
+      <c r="A39" s="74"/>
       <c r="B39" s="33">
         <v>20</v>
       </c>
@@ -1996,30 +2010,31 @@
       </c>
     </row>
     <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A40" s="89"/>
-      <c r="B40" s="78" t="s">
+      <c r="A40" s="56"/>
+      <c r="B40" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="78"/>
-      <c r="I40" s="95"/>
+      <c r="C40" s="65"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="66"/>
     </row>
     <row r="41" spans="1:9" s="16" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="89"/>
+      <c r="A41" s="56"/>
       <c r="B41" s="18"/>
       <c r="C41" s="17">
-        <v>27</v>
+        <f>COUNTIF(C4:C39, "&lt;&gt;")</f>
+        <v>24</v>
       </c>
       <c r="D41" s="17">
-        <f t="shared" ref="D41:I41" si="0">COUNTIF(D4:D39, "&lt;&gt;")</f>
-        <v>19</v>
+        <f>COUNTIF(D4:D39, "&lt;&gt;")</f>
+        <v>20</v>
       </c>
       <c r="E41" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D41:I41" si="0">COUNTIF(E4:E39, "&lt;&gt;")</f>
         <v>9</v>
       </c>
       <c r="F41" s="17">
@@ -2040,36 +2055,88 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="89"/>
-      <c r="B42" s="78" t="str">
+      <c r="A42" s="56"/>
+      <c r="B42" s="65" t="str">
         <f>SUM(C41:I41) &amp; " Total Races (Prior to Breeders' Cup Weekend)"</f>
-        <v>98 Total Races (Prior to Breeders' Cup Weekend)</v>
-      </c>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78"/>
-      <c r="I42" s="78"/>
+        <v>96 Total Races (Prior to Breeders' Cup Weekend)</v>
+      </c>
+      <c r="C42" s="65"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="65"/>
     </row>
     <row r="43" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="89"/>
-      <c r="B43" s="90" t="s">
+      <c r="A43" s="56"/>
+      <c r="B43" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="90"/>
-      <c r="D43" s="90"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="92" t="s">
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="94"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
+  <mergeCells count="68">
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="I36:I38"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="H32:H35"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="F4:F6"/>
@@ -2081,70 +2148,11 @@
     <mergeCell ref="G32:G35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="C1:I1"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="F14:F16"/>
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="A2:A39"/>
     <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="G36:G38"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="I36:I38"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="H32:H35"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="G30:G31"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>